<commit_message>
First Model to reviez
</commit_message>
<xml_diff>
--- a/HousingData.xlsx
+++ b/HousingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/My Drive (victorr@mit.edu)/Documents importants/Academic/MIT/Fall/15_093_Optimization/Project/OptimizationProject_DARP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B933A6-A42A-3F4E-A279-F1FCC97C1190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D9C79D-1FCE-3C47-B635-27CA81C99946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="20040" xr2:uid="{7B6ADF93-13BD-7441-8FE5-7B1CCF4DC47D}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{7B6ADF93-13BD-7441-8FE5-7B1CCF4DC47D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -906,9 +906,6 @@
       <c r="E18" t="s">
         <v>29</v>
       </c>
-      <c r="F18">
-        <v>100</v>
-      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -926,9 +923,6 @@
       <c r="E19" t="s">
         <v>29</v>
       </c>
-      <c r="F19">
-        <v>100</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -946,9 +940,6 @@
       <c r="E20" t="s">
         <v>29</v>
       </c>
-      <c r="F20">
-        <v>100</v>
-      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -965,9 +956,6 @@
       </c>
       <c r="E21" t="s">
         <v>29</v>
-      </c>
-      <c r="F21">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Real Data Generation + Model trained on it
</commit_message>
<xml_diff>
--- a/HousingData.xlsx
+++ b/HousingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/My Drive (victorr@mit.edu)/Documents importants/Academic/MIT/Fall/15_093_Optimization/Project/OptimizationProject_DARP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3B88A2-26E0-264A-9065-CB704E5EF9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BF5B93-2BE1-C542-88D4-90E50A9656F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{7B6ADF93-13BD-7441-8FE5-7B1CCF4DC47D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{7B6ADF93-13BD-7441-8FE5-7B1CCF4DC47D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -906,6 +906,9 @@
       <c r="E18" t="s">
         <v>29</v>
       </c>
+      <c r="F18">
+        <v>1285</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -923,6 +926,9 @@
       <c r="E19" t="s">
         <v>29</v>
       </c>
+      <c r="F19">
+        <v>120</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -940,6 +946,9 @@
       <c r="E20" t="s">
         <v>29</v>
       </c>
+      <c r="F20">
+        <v>266</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -956,6 +965,9 @@
       </c>
       <c r="E21" t="s">
         <v>29</v>
+      </c>
+      <c r="F21">
+        <v>832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>